<commit_message>
[Q3] Update list to contain only carparks to keep
</commit_message>
<xml_diff>
--- a/Question 3/Carparks_Keep_Throw_List.xlsx
+++ b/Question 3/Carparks_Keep_Throw_List.xlsx
@@ -5,16 +5,19 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ramana/Desktop/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://nusu-my.sharepoint.com/personal/e0398581_u_nus_edu/Documents/Uni/NUS/Year 4/Y4S1/EE4211/Project/Github Repo/EE4211-Project/Question 3/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{9DB683ED-EB65-F743-B34A-027D6D9A76AD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="5" documentId="8_{9DB683ED-EB65-F743-B34A-027D6D9A76AD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{DF8CEBD3-9B72-454B-9E16-301414AA6BD0}"/>
   <bookViews>
-    <workbookView xWindow="29400" yWindow="500" windowWidth="25600" windowHeight="28300" xr2:uid="{BFADA698-3CF4-8F4C-AEA4-703DB845C86C}"/>
+    <workbookView xWindow="0" yWindow="740" windowWidth="29400" windowHeight="18380" xr2:uid="{BFADA698-3CF4-8F4C-AEA4-703DB845C86C}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$B$1:$B$154</definedName>
+  </definedNames>
   <calcPr calcId="181029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -36,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="354" uniqueCount="180">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="308" uniqueCount="156">
   <si>
     <t>Carpark</t>
   </si>
@@ -50,12 +53,6 @@
     <t>Keep</t>
   </si>
   <si>
-    <t>DWST</t>
-  </si>
-  <si>
-    <t>Throw</t>
-  </si>
-  <si>
     <t>DWSV</t>
   </si>
   <si>
@@ -119,27 +116,18 @@
     <t>HCM</t>
   </si>
   <si>
-    <t>HE1</t>
-  </si>
-  <si>
     <t>HE12</t>
   </si>
   <si>
     <t>HE17</t>
   </si>
   <si>
-    <t>HE19</t>
-  </si>
-  <si>
     <t>HE24</t>
   </si>
   <si>
     <t>HE3</t>
   </si>
   <si>
-    <t>HE4</t>
-  </si>
-  <si>
     <t>HE9</t>
   </si>
   <si>
@@ -158,9 +146,6 @@
     <t>JBM2</t>
   </si>
   <si>
-    <t>JKM</t>
-  </si>
-  <si>
     <t>JKS</t>
   </si>
   <si>
@@ -197,21 +182,12 @@
     <t>KTM4</t>
   </si>
   <si>
-    <t>KTM5</t>
-  </si>
-  <si>
     <t>LBM</t>
   </si>
   <si>
-    <t>MLM</t>
-  </si>
-  <si>
     <t>MLM1</t>
   </si>
   <si>
-    <t>PDQ5</t>
-  </si>
-  <si>
     <t>PRM</t>
   </si>
   <si>
@@ -281,9 +257,6 @@
     <t>Q94</t>
   </si>
   <si>
-    <t>Q96</t>
-  </si>
-  <si>
     <t>RHM</t>
   </si>
   <si>
@@ -296,9 +269,6 @@
     <t>RHM4</t>
   </si>
   <si>
-    <t>RHS</t>
-  </si>
-  <si>
     <t>SAM</t>
   </si>
   <si>
@@ -308,12 +278,6 @@
     <t>SLS</t>
   </si>
   <si>
-    <t>SMM</t>
-  </si>
-  <si>
-    <t>SPM</t>
-  </si>
-  <si>
     <t>SPS</t>
   </si>
   <si>
@@ -326,15 +290,9 @@
     <t>STM2</t>
   </si>
   <si>
-    <t>STM3</t>
-  </si>
-  <si>
     <t>TB1</t>
   </si>
   <si>
-    <t>TB10</t>
-  </si>
-  <si>
     <t>TB11</t>
   </si>
   <si>
@@ -356,33 +314,21 @@
     <t>TB22</t>
   </si>
   <si>
-    <t>TB23</t>
-  </si>
-  <si>
     <t>TB28</t>
   </si>
   <si>
     <t>TB3</t>
   </si>
   <si>
-    <t>TB6</t>
-  </si>
-  <si>
     <t>TB7</t>
   </si>
   <si>
-    <t>TB8</t>
-  </si>
-  <si>
     <t>TB9</t>
   </si>
   <si>
     <t>TBC2</t>
   </si>
   <si>
-    <t>TBC3</t>
-  </si>
-  <si>
     <t>TBCM</t>
   </si>
   <si>
@@ -392,9 +338,6 @@
     <t>TBM</t>
   </si>
   <si>
-    <t>TBM2</t>
-  </si>
-  <si>
     <t>TBM3</t>
   </si>
   <si>
@@ -431,9 +374,6 @@
     <t>TE25</t>
   </si>
   <si>
-    <t>TE3</t>
-  </si>
-  <si>
     <t>TE4</t>
   </si>
   <si>
@@ -563,19 +503,10 @@
     <t>DRS</t>
   </si>
   <si>
-    <t>DSR1</t>
-  </si>
-  <si>
-    <t>DSR2</t>
-  </si>
-  <si>
     <t>DSRL</t>
   </si>
   <si>
     <t>DUXM</t>
-  </si>
-  <si>
-    <t>SWS0</t>
   </si>
 </sst>
 </file>
@@ -637,6 +568,10 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -936,10 +871,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EAEEFCA0-15EC-1C4B-AEE0-DD030AEF6E04}">
-  <dimension ref="A1:B177"/>
+  <dimension ref="A1:B154"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A46" sqref="A46"/>
+    <sheetView tabSelected="1" topLeftCell="A144" workbookViewId="0">
+      <selection activeCell="E29" sqref="E29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -954,7 +889,7 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>136</v>
+        <v>115</v>
       </c>
       <c r="B2" t="s">
         <v>3</v>
@@ -962,7 +897,7 @@
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>137</v>
+        <v>116</v>
       </c>
       <c r="B3" t="s">
         <v>3</v>
@@ -970,7 +905,7 @@
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>138</v>
+        <v>117</v>
       </c>
       <c r="B4" t="s">
         <v>3</v>
@@ -978,7 +913,7 @@
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>139</v>
+        <v>118</v>
       </c>
       <c r="B5" t="s">
         <v>3</v>
@@ -986,7 +921,7 @@
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>140</v>
+        <v>119</v>
       </c>
       <c r="B6" t="s">
         <v>3</v>
@@ -994,7 +929,7 @@
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>141</v>
+        <v>120</v>
       </c>
       <c r="B7" t="s">
         <v>3</v>
@@ -1002,7 +937,7 @@
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>142</v>
+        <v>121</v>
       </c>
       <c r="B8" t="s">
         <v>3</v>
@@ -1010,7 +945,7 @@
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>143</v>
+        <v>122</v>
       </c>
       <c r="B9" t="s">
         <v>3</v>
@@ -1018,7 +953,7 @@
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>144</v>
+        <v>123</v>
       </c>
       <c r="B10" t="s">
         <v>3</v>
@@ -1026,7 +961,7 @@
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>145</v>
+        <v>124</v>
       </c>
       <c r="B11" t="s">
         <v>3</v>
@@ -1034,7 +969,7 @@
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>146</v>
+        <v>125</v>
       </c>
       <c r="B12" t="s">
         <v>3</v>
@@ -1042,7 +977,7 @@
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>147</v>
+        <v>126</v>
       </c>
       <c r="B13" t="s">
         <v>3</v>
@@ -1050,7 +985,7 @@
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>148</v>
+        <v>127</v>
       </c>
       <c r="B14" t="s">
         <v>3</v>
@@ -1058,7 +993,7 @@
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>149</v>
+        <v>128</v>
       </c>
       <c r="B15" t="s">
         <v>3</v>
@@ -1066,7 +1001,7 @@
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>150</v>
+        <v>129</v>
       </c>
       <c r="B16" t="s">
         <v>3</v>
@@ -1074,7 +1009,7 @@
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>151</v>
+        <v>130</v>
       </c>
       <c r="B17" t="s">
         <v>3</v>
@@ -1082,7 +1017,7 @@
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>152</v>
+        <v>131</v>
       </c>
       <c r="B18" t="s">
         <v>3</v>
@@ -1090,7 +1025,7 @@
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
-        <v>153</v>
+        <v>132</v>
       </c>
       <c r="B19" t="s">
         <v>3</v>
@@ -1098,7 +1033,7 @@
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
-        <v>154</v>
+        <v>133</v>
       </c>
       <c r="B20" t="s">
         <v>3</v>
@@ -1106,7 +1041,7 @@
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
-        <v>155</v>
+        <v>134</v>
       </c>
       <c r="B21" t="s">
         <v>3</v>
@@ -1114,7 +1049,7 @@
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
-        <v>156</v>
+        <v>135</v>
       </c>
       <c r="B22" t="s">
         <v>3</v>
@@ -1122,7 +1057,7 @@
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
-        <v>157</v>
+        <v>136</v>
       </c>
       <c r="B23" t="s">
         <v>3</v>
@@ -1130,7 +1065,7 @@
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
-        <v>158</v>
+        <v>137</v>
       </c>
       <c r="B24" t="s">
         <v>3</v>
@@ -1138,7 +1073,7 @@
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
-        <v>159</v>
+        <v>138</v>
       </c>
       <c r="B25" t="s">
         <v>3</v>
@@ -1146,7 +1081,7 @@
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
-        <v>160</v>
+        <v>139</v>
       </c>
       <c r="B26" t="s">
         <v>3</v>
@@ -1154,7 +1089,7 @@
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
-        <v>161</v>
+        <v>140</v>
       </c>
       <c r="B27" t="s">
         <v>3</v>
@@ -1162,7 +1097,7 @@
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
-        <v>162</v>
+        <v>141</v>
       </c>
       <c r="B28" t="s">
         <v>3</v>
@@ -1170,7 +1105,7 @@
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
-        <v>163</v>
+        <v>142</v>
       </c>
       <c r="B29" t="s">
         <v>3</v>
@@ -1178,7 +1113,7 @@
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
-        <v>164</v>
+        <v>143</v>
       </c>
       <c r="B30" t="s">
         <v>3</v>
@@ -1186,7 +1121,7 @@
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
-        <v>165</v>
+        <v>144</v>
       </c>
       <c r="B31" t="s">
         <v>3</v>
@@ -1194,7 +1129,7 @@
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
-        <v>166</v>
+        <v>145</v>
       </c>
       <c r="B32" t="s">
         <v>3</v>
@@ -1202,7 +1137,7 @@
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
-        <v>167</v>
+        <v>146</v>
       </c>
       <c r="B33" t="s">
         <v>3</v>
@@ -1210,7 +1145,7 @@
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
-        <v>168</v>
+        <v>147</v>
       </c>
       <c r="B34" t="s">
         <v>3</v>
@@ -1218,7 +1153,7 @@
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
-        <v>169</v>
+        <v>148</v>
       </c>
       <c r="B35" t="s">
         <v>3</v>
@@ -1226,7 +1161,7 @@
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
-        <v>170</v>
+        <v>149</v>
       </c>
       <c r="B36" t="s">
         <v>3</v>
@@ -1234,7 +1169,7 @@
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
-        <v>171</v>
+        <v>150</v>
       </c>
       <c r="B37" t="s">
         <v>3</v>
@@ -1242,7 +1177,7 @@
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
-        <v>172</v>
+        <v>151</v>
       </c>
       <c r="B38" t="s">
         <v>3</v>
@@ -1250,7 +1185,7 @@
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
-        <v>173</v>
+        <v>152</v>
       </c>
       <c r="B39" t="s">
         <v>3</v>
@@ -1258,7 +1193,7 @@
     </row>
     <row r="40" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
-        <v>174</v>
+        <v>153</v>
       </c>
       <c r="B40" t="s">
         <v>3</v>
@@ -1266,23 +1201,23 @@
     </row>
     <row r="41" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
-        <v>175</v>
+        <v>154</v>
       </c>
       <c r="B41" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
     </row>
     <row r="42" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
-        <v>176</v>
+        <v>155</v>
       </c>
       <c r="B42" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
     </row>
     <row r="43" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
-        <v>177</v>
+        <v>2</v>
       </c>
       <c r="B43" t="s">
         <v>3</v>
@@ -1290,7 +1225,7 @@
     </row>
     <row r="44" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
-        <v>178</v>
+        <v>4</v>
       </c>
       <c r="B44" t="s">
         <v>3</v>
@@ -1298,15 +1233,15 @@
     </row>
     <row r="45" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
-        <v>179</v>
+        <v>5</v>
       </c>
       <c r="B45" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
     </row>
     <row r="46" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="B46" t="s">
         <v>3</v>
@@ -1314,15 +1249,15 @@
     </row>
     <row r="47" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="B47" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
     </row>
     <row r="48" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="B48" t="s">
         <v>3</v>
@@ -1330,7 +1265,7 @@
     </row>
     <row r="49" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="B49" t="s">
         <v>3</v>
@@ -1338,7 +1273,7 @@
     </row>
     <row r="50" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="B50" t="s">
         <v>3</v>
@@ -1346,7 +1281,7 @@
     </row>
     <row r="51" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A51" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="B51" t="s">
         <v>3</v>
@@ -1354,7 +1289,7 @@
     </row>
     <row r="52" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A52" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="B52" t="s">
         <v>3</v>
@@ -1362,7 +1297,7 @@
     </row>
     <row r="53" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A53" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="B53" t="s">
         <v>3</v>
@@ -1370,7 +1305,7 @@
     </row>
     <row r="54" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A54" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="B54" t="s">
         <v>3</v>
@@ -1378,7 +1313,7 @@
     </row>
     <row r="55" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A55" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="B55" t="s">
         <v>3</v>
@@ -1386,7 +1321,7 @@
     </row>
     <row r="56" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A56" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="B56" t="s">
         <v>3</v>
@@ -1394,7 +1329,7 @@
     </row>
     <row r="57" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A57" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="B57" t="s">
         <v>3</v>
@@ -1402,7 +1337,7 @@
     </row>
     <row r="58" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A58" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="B58" t="s">
         <v>3</v>
@@ -1410,7 +1345,7 @@
     </row>
     <row r="59" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A59" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="B59" t="s">
         <v>3</v>
@@ -1418,7 +1353,7 @@
     </row>
     <row r="60" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A60" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="B60" t="s">
         <v>3</v>
@@ -1426,7 +1361,7 @@
     </row>
     <row r="61" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A61" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="B61" t="s">
         <v>3</v>
@@ -1434,7 +1369,7 @@
     </row>
     <row r="62" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A62" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="B62" t="s">
         <v>3</v>
@@ -1442,7 +1377,7 @@
     </row>
     <row r="63" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A63" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="B63" t="s">
         <v>3</v>
@@ -1450,7 +1385,7 @@
     </row>
     <row r="64" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A64" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="B64" t="s">
         <v>3</v>
@@ -1458,7 +1393,7 @@
     </row>
     <row r="65" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A65" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="B65" t="s">
         <v>3</v>
@@ -1466,7 +1401,7 @@
     </row>
     <row r="66" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A66" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="B66" t="s">
         <v>3</v>
@@ -1474,7 +1409,7 @@
     </row>
     <row r="67" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A67" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="B67" t="s">
         <v>3</v>
@@ -1482,7 +1417,7 @@
     </row>
     <row r="68" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A68" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="B68" t="s">
         <v>3</v>
@@ -1490,15 +1425,15 @@
     </row>
     <row r="69" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A69" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="B69" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
     </row>
     <row r="70" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A70" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="B70" t="s">
         <v>3</v>
@@ -1506,7 +1441,7 @@
     </row>
     <row r="71" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A71" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="B71" t="s">
         <v>3</v>
@@ -1514,15 +1449,15 @@
     </row>
     <row r="72" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A72" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="B72" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
     </row>
     <row r="73" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A73" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="B73" t="s">
         <v>3</v>
@@ -1530,7 +1465,7 @@
     </row>
     <row r="74" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A74" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="B74" t="s">
         <v>3</v>
@@ -1538,15 +1473,15 @@
     </row>
     <row r="75" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A75" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="B75" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
     </row>
     <row r="76" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A76" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="B76" t="s">
         <v>3</v>
@@ -1554,7 +1489,7 @@
     </row>
     <row r="77" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A77" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="B77" t="s">
         <v>3</v>
@@ -1562,7 +1497,7 @@
     </row>
     <row r="78" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A78" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="B78" t="s">
         <v>3</v>
@@ -1570,7 +1505,7 @@
     </row>
     <row r="79" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A79" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="B79" t="s">
         <v>3</v>
@@ -1578,7 +1513,7 @@
     </row>
     <row r="80" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A80" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="B80" t="s">
         <v>3</v>
@@ -1586,7 +1521,7 @@
     </row>
     <row r="81" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A81" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="B81" t="s">
         <v>3</v>
@@ -1594,15 +1529,15 @@
     </row>
     <row r="82" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A82" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="B82" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
     </row>
     <row r="83" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A83" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="B83" t="s">
         <v>3</v>
@@ -1610,7 +1545,7 @@
     </row>
     <row r="84" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A84" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="B84" t="s">
         <v>3</v>
@@ -1618,7 +1553,7 @@
     </row>
     <row r="85" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A85" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="B85" t="s">
         <v>3</v>
@@ -1626,7 +1561,7 @@
     </row>
     <row r="86" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A86" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="B86" t="s">
         <v>3</v>
@@ -1634,7 +1569,7 @@
     </row>
     <row r="87" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A87" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="B87" t="s">
         <v>3</v>
@@ -1642,7 +1577,7 @@
     </row>
     <row r="88" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A88" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="B88" t="s">
         <v>3</v>
@@ -1650,7 +1585,7 @@
     </row>
     <row r="89" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A89" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="B89" t="s">
         <v>3</v>
@@ -1658,7 +1593,7 @@
     </row>
     <row r="90" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A90" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="B90" t="s">
         <v>3</v>
@@ -1666,7 +1601,7 @@
     </row>
     <row r="91" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A91" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="B91" t="s">
         <v>3</v>
@@ -1674,7 +1609,7 @@
     </row>
     <row r="92" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A92" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="B92" t="s">
         <v>3</v>
@@ -1682,7 +1617,7 @@
     </row>
     <row r="93" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A93" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="B93" t="s">
         <v>3</v>
@@ -1690,7 +1625,7 @@
     </row>
     <row r="94" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A94" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="B94" t="s">
         <v>3</v>
@@ -1698,15 +1633,15 @@
     </row>
     <row r="95" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A95" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="B95" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
     </row>
     <row r="96" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A96" t="s">
-        <v>54</v>
+        <v>56</v>
       </c>
       <c r="B96" t="s">
         <v>3</v>
@@ -1714,15 +1649,15 @@
     </row>
     <row r="97" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A97" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="B97" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
     </row>
     <row r="98" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A98" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="B98" t="s">
         <v>3</v>
@@ -1730,15 +1665,15 @@
     </row>
     <row r="99" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A99" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="B99" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
     </row>
     <row r="100" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A100" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="B100" t="s">
         <v>3</v>
@@ -1746,7 +1681,7 @@
     </row>
     <row r="101" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A101" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
       <c r="B101" t="s">
         <v>3</v>
@@ -1754,7 +1689,7 @@
     </row>
     <row r="102" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A102" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="B102" t="s">
         <v>3</v>
@@ -1762,7 +1697,7 @@
     </row>
     <row r="103" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A103" t="s">
-        <v>61</v>
+        <v>63</v>
       </c>
       <c r="B103" t="s">
         <v>3</v>
@@ -1770,7 +1705,7 @@
     </row>
     <row r="104" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A104" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="B104" t="s">
         <v>3</v>
@@ -1778,7 +1713,7 @@
     </row>
     <row r="105" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A105" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="B105" t="s">
         <v>3</v>
@@ -1786,7 +1721,7 @@
     </row>
     <row r="106" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A106" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="B106" t="s">
         <v>3</v>
@@ -1794,7 +1729,7 @@
     </row>
     <row r="107" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A107" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
       <c r="B107" t="s">
         <v>3</v>
@@ -1802,7 +1737,7 @@
     </row>
     <row r="108" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A108" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="B108" t="s">
         <v>3</v>
@@ -1810,7 +1745,7 @@
     </row>
     <row r="109" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A109" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="B109" t="s">
         <v>3</v>
@@ -1818,7 +1753,7 @@
     </row>
     <row r="110" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A110" t="s">
-        <v>68</v>
+        <v>70</v>
       </c>
       <c r="B110" t="s">
         <v>3</v>
@@ -1826,7 +1761,7 @@
     </row>
     <row r="111" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A111" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
       <c r="B111" t="s">
         <v>3</v>
@@ -1834,7 +1769,7 @@
     </row>
     <row r="112" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A112" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="B112" t="s">
         <v>3</v>
@@ -1842,7 +1777,7 @@
     </row>
     <row r="113" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A113" t="s">
-        <v>71</v>
+        <v>73</v>
       </c>
       <c r="B113" t="s">
         <v>3</v>
@@ -1850,7 +1785,7 @@
     </row>
     <row r="114" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A114" t="s">
-        <v>72</v>
+        <v>74</v>
       </c>
       <c r="B114" t="s">
         <v>3</v>
@@ -1858,7 +1793,7 @@
     </row>
     <row r="115" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A115" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="B115" t="s">
         <v>3</v>
@@ -1866,7 +1801,7 @@
     </row>
     <row r="116" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A116" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="B116" t="s">
         <v>3</v>
@@ -1874,7 +1809,7 @@
     </row>
     <row r="117" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A117" t="s">
-        <v>75</v>
+        <v>77</v>
       </c>
       <c r="B117" t="s">
         <v>3</v>
@@ -1882,7 +1817,7 @@
     </row>
     <row r="118" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A118" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
       <c r="B118" t="s">
         <v>3</v>
@@ -1890,7 +1825,7 @@
     </row>
     <row r="119" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A119" t="s">
-        <v>77</v>
+        <v>79</v>
       </c>
       <c r="B119" t="s">
         <v>3</v>
@@ -1898,7 +1833,7 @@
     </row>
     <row r="120" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A120" t="s">
-        <v>78</v>
+        <v>80</v>
       </c>
       <c r="B120" t="s">
         <v>3</v>
@@ -1906,7 +1841,7 @@
     </row>
     <row r="121" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A121" t="s">
-        <v>79</v>
+        <v>81</v>
       </c>
       <c r="B121" t="s">
         <v>3</v>
@@ -1914,7 +1849,7 @@
     </row>
     <row r="122" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A122" t="s">
-        <v>80</v>
+        <v>82</v>
       </c>
       <c r="B122" t="s">
         <v>3</v>
@@ -1922,15 +1857,15 @@
     </row>
     <row r="123" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A123" t="s">
-        <v>81</v>
+        <v>83</v>
       </c>
       <c r="B123" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
     </row>
     <row r="124" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A124" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="B124" t="s">
         <v>3</v>
@@ -1938,7 +1873,7 @@
     </row>
     <row r="125" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A125" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
       <c r="B125" t="s">
         <v>3</v>
@@ -1946,7 +1881,7 @@
     </row>
     <row r="126" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A126" t="s">
-        <v>84</v>
+        <v>86</v>
       </c>
       <c r="B126" t="s">
         <v>3</v>
@@ -1954,7 +1889,7 @@
     </row>
     <row r="127" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A127" t="s">
-        <v>85</v>
+        <v>87</v>
       </c>
       <c r="B127" t="s">
         <v>3</v>
@@ -1962,15 +1897,15 @@
     </row>
     <row r="128" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A128" t="s">
-        <v>86</v>
+        <v>88</v>
       </c>
       <c r="B128" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
     </row>
     <row r="129" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A129" t="s">
-        <v>87</v>
+        <v>89</v>
       </c>
       <c r="B129" t="s">
         <v>3</v>
@@ -1978,7 +1913,7 @@
     </row>
     <row r="130" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A130" t="s">
-        <v>88</v>
+        <v>90</v>
       </c>
       <c r="B130" t="s">
         <v>3</v>
@@ -1986,7 +1921,7 @@
     </row>
     <row r="131" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A131" t="s">
-        <v>89</v>
+        <v>91</v>
       </c>
       <c r="B131" t="s">
         <v>3</v>
@@ -1994,23 +1929,23 @@
     </row>
     <row r="132" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A132" t="s">
-        <v>90</v>
+        <v>92</v>
       </c>
       <c r="B132" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
     </row>
     <row r="133" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A133" t="s">
-        <v>91</v>
+        <v>93</v>
       </c>
       <c r="B133" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
     </row>
     <row r="134" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A134" t="s">
-        <v>92</v>
+        <v>94</v>
       </c>
       <c r="B134" t="s">
         <v>3</v>
@@ -2018,7 +1953,7 @@
     </row>
     <row r="135" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A135" t="s">
-        <v>93</v>
+        <v>95</v>
       </c>
       <c r="B135" t="s">
         <v>3</v>
@@ -2026,7 +1961,7 @@
     </row>
     <row r="136" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A136" t="s">
-        <v>94</v>
+        <v>96</v>
       </c>
       <c r="B136" t="s">
         <v>3</v>
@@ -2034,7 +1969,7 @@
     </row>
     <row r="137" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A137" t="s">
-        <v>95</v>
+        <v>97</v>
       </c>
       <c r="B137" t="s">
         <v>3</v>
@@ -2042,15 +1977,15 @@
     </row>
     <row r="138" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A138" t="s">
-        <v>96</v>
+        <v>98</v>
       </c>
       <c r="B138" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
     </row>
     <row r="139" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A139" t="s">
-        <v>97</v>
+        <v>99</v>
       </c>
       <c r="B139" t="s">
         <v>3</v>
@@ -2058,15 +1993,15 @@
     </row>
     <row r="140" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A140" t="s">
-        <v>98</v>
+        <v>100</v>
       </c>
       <c r="B140" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
     </row>
     <row r="141" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A141" t="s">
-        <v>99</v>
+        <v>101</v>
       </c>
       <c r="B141" t="s">
         <v>3</v>
@@ -2074,7 +2009,7 @@
     </row>
     <row r="142" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A142" t="s">
-        <v>100</v>
+        <v>102</v>
       </c>
       <c r="B142" t="s">
         <v>3</v>
@@ -2082,7 +2017,7 @@
     </row>
     <row r="143" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A143" t="s">
-        <v>101</v>
+        <v>103</v>
       </c>
       <c r="B143" t="s">
         <v>3</v>
@@ -2090,7 +2025,7 @@
     </row>
     <row r="144" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A144" t="s">
-        <v>102</v>
+        <v>104</v>
       </c>
       <c r="B144" t="s">
         <v>3</v>
@@ -2098,7 +2033,7 @@
     </row>
     <row r="145" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A145" t="s">
-        <v>103</v>
+        <v>105</v>
       </c>
       <c r="B145" t="s">
         <v>3</v>
@@ -2106,7 +2041,7 @@
     </row>
     <row r="146" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A146" t="s">
-        <v>104</v>
+        <v>106</v>
       </c>
       <c r="B146" t="s">
         <v>3</v>
@@ -2114,7 +2049,7 @@
     </row>
     <row r="147" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A147" t="s">
-        <v>105</v>
+        <v>107</v>
       </c>
       <c r="B147" t="s">
         <v>3</v>
@@ -2122,15 +2057,15 @@
     </row>
     <row r="148" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A148" t="s">
-        <v>106</v>
+        <v>108</v>
       </c>
       <c r="B148" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
     </row>
     <row r="149" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A149" t="s">
-        <v>107</v>
+        <v>109</v>
       </c>
       <c r="B149" t="s">
         <v>3</v>
@@ -2138,7 +2073,7 @@
     </row>
     <row r="150" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A150" t="s">
-        <v>108</v>
+        <v>110</v>
       </c>
       <c r="B150" t="s">
         <v>3</v>
@@ -2146,15 +2081,15 @@
     </row>
     <row r="151" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A151" t="s">
-        <v>109</v>
+        <v>111</v>
       </c>
       <c r="B151" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
     </row>
     <row r="152" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A152" t="s">
-        <v>110</v>
+        <v>112</v>
       </c>
       <c r="B152" t="s">
         <v>3</v>
@@ -2162,205 +2097,22 @@
     </row>
     <row r="153" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A153" t="s">
-        <v>111</v>
+        <v>113</v>
       </c>
       <c r="B153" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
     </row>
     <row r="154" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A154" t="s">
-        <v>112</v>
+        <v>114</v>
       </c>
       <c r="B154" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="155" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A155" t="s">
-        <v>113</v>
-      </c>
-      <c r="B155" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="156" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A156" t="s">
-        <v>114</v>
-      </c>
-      <c r="B156" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="157" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A157" t="s">
-        <v>115</v>
-      </c>
-      <c r="B157" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="158" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A158" t="s">
-        <v>116</v>
-      </c>
-      <c r="B158" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="159" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A159" t="s">
-        <v>117</v>
-      </c>
-      <c r="B159" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="160" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A160" t="s">
-        <v>118</v>
-      </c>
-      <c r="B160" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="161" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A161" t="s">
-        <v>119</v>
-      </c>
-      <c r="B161" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="162" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A162" t="s">
-        <v>120</v>
-      </c>
-      <c r="B162" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="163" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A163" t="s">
-        <v>121</v>
-      </c>
-      <c r="B163" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="164" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A164" t="s">
-        <v>122</v>
-      </c>
-      <c r="B164" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="165" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A165" t="s">
-        <v>123</v>
-      </c>
-      <c r="B165" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="166" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A166" t="s">
-        <v>124</v>
-      </c>
-      <c r="B166" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="167" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A167" t="s">
-        <v>125</v>
-      </c>
-      <c r="B167" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="168" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A168" t="s">
-        <v>126</v>
-      </c>
-      <c r="B168" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="169" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A169" t="s">
-        <v>127</v>
-      </c>
-      <c r="B169" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="170" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A170" t="s">
-        <v>128</v>
-      </c>
-      <c r="B170" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="171" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A171" t="s">
-        <v>129</v>
-      </c>
-      <c r="B171" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="172" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A172" t="s">
-        <v>130</v>
-      </c>
-      <c r="B172" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="173" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A173" t="s">
-        <v>131</v>
-      </c>
-      <c r="B173" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="174" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A174" t="s">
-        <v>132</v>
-      </c>
-      <c r="B174" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="175" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A175" t="s">
-        <v>133</v>
-      </c>
-      <c r="B175" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="176" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A176" t="s">
-        <v>134</v>
-      </c>
-      <c r="B176" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="177" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A177" t="s">
-        <v>135</v>
-      </c>
-      <c r="B177" t="s">
-        <v>3</v>
-      </c>
-    </row>
   </sheetData>
+  <autoFilter ref="B1:B154" xr:uid="{EAEEFCA0-15EC-1C4B-AEE0-DD030AEF6E04}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>